<commit_message>
my algorithm + gamesplits class
</commit_message>
<xml_diff>
--- a/__data__/betting_data.xlsx
+++ b/__data__/betting_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobyhoffman/PycharmProjects/SCQ-Comp/SCQ-Betting/__data__/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rileyheike/Desktop/SCQ-Betting/__data__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6C2179-A3CA-A541-AF37-C54FA0A587E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F672E9A-17E7-894A-836A-67953E032E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="760" windowWidth="28300" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="880" windowWidth="12800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Team 1</t>
   </si>
@@ -34,70 +34,16 @@
     <t>Total Points</t>
   </si>
   <si>
-    <t>+2.5</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>+5.5</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>+1</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
     <t>ML1</t>
   </si>
   <si>
     <t>ML2</t>
   </si>
   <si>
-    <t>CLE</t>
-  </si>
-  <si>
-    <t>NYK</t>
-  </si>
-  <si>
-    <t>DEN</t>
-  </si>
-  <si>
-    <t>LAL</t>
-  </si>
-  <si>
-    <t>PHI</t>
-  </si>
-  <si>
-    <t>ORL</t>
-  </si>
-  <si>
-    <t>MIL</t>
-  </si>
-  <si>
-    <t>IND</t>
-  </si>
-  <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>PHO</t>
-  </si>
-  <si>
-    <t>MIA</t>
-  </si>
-  <si>
-    <t>BOS</t>
-  </si>
-  <si>
     <t>DAL</t>
   </si>
   <si>
-    <t>LAC</t>
+    <t>OKC</t>
   </si>
 </sst>
 </file>
@@ -154,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -162,7 +108,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +413,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,10 +426,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -495,143 +440,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="D2" s="2">
-        <v>-135</v>
-      </c>
-      <c r="E2" t="s">
+        <v>-180</v>
+      </c>
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
+      <c r="F2">
+        <v>207.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2">
-        <v>195</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-238</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-105</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-115</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>114</v>
-      </c>
-      <c r="D5">
-        <v>-135</v>
-      </c>
-      <c r="E5" s="3">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>216.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>195</v>
-      </c>
-      <c r="D6">
-        <v>-238</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>213</v>
-      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2">
-        <v>300</v>
-      </c>
-      <c r="D7" s="2">
-        <v>-250</v>
-      </c>
-      <c r="E7" s="3">
-        <v>19.5</v>
-      </c>
-      <c r="F7">
-        <v>208.5</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-148</v>
-      </c>
-      <c r="D8" s="2">
-        <v>124</v>
-      </c>
-      <c r="E8">
-        <v>-3</v>
-      </c>
-      <c r="F8">
-        <v>209</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>